<commit_message>
refact login page automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -4,48 +4,47 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="5715" windowWidth="12765" xWindow="0" yWindow="105"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715"/>
   </bookViews>
   <sheets>
-    <sheet name="testData" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="testData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Test Case Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UserName</t>
+    <t>TrainScheduling_ltrailways_login_master</t>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_login_master</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Password</t>
+    <t>Login.login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Results</t>
+    <t>password</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test01</t>
+    <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -61,15 +60,27 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,19 +88,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -98,10 +134,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -257,7 +293,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -266,13 +302,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -282,7 +318,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -291,7 +327,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -300,7 +336,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -310,12 +346,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -346,7 +382,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -365,7 +401,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -378,51 +414,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="16.0" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="16.5" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="9.125" collapsed="false"/>
-    <col min="4" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="1" width="35.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.95" customHeight="1"/>
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="D3" s="3">
         <v>13659191907</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E3" s="3">
         <v>654321</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
+      <c r="F3" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -435,7 +481,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -448,6 +494,6 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1.refactor script; 2.add logout script; 3.add 'add company' script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,6 +39,30 @@
   </si>
   <si>
     <t>TrainScheduling_ltrailways_login_master</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_addCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>companyName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xuliangTested</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forTesting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComanyManagemetn.addCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>detailsOfCompany</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,19 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -466,6 +490,41 @@
         <v>654321</v>
       </c>
       <c r="F3" s="5"/>
+    </row>
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
refactor add company automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,15 +54,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>forTesting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ComanyManagemetn.addCompany</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>detailsOfCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>james</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">company details </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -442,7 +450,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -483,11 +491,11 @@
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3">
-        <v>13659191907</v>
-      </c>
-      <c r="E3" s="3">
-        <v>654321</v>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -499,13 +507,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="15.95" customHeight="1">
@@ -516,13 +524,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F6" s="5"/>
     </row>

</xml_diff>

<commit_message>
add add_Department automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +71,34 @@
   </si>
   <si>
     <t xml:space="preserve">company details </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_addDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComanyManagemetn.addDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComanyManagemetn.addDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>departmentName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_generated_DN </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_generated_CD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -459,8 +487,9 @@
     <col min="2" max="2" width="4" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="19.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="15.95" customHeight="1"/>
@@ -533,6 +562,46 @@
         <v>13</v>
       </c>
       <c r="F6" s="5"/>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add 'update_company' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,10 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ComanyManagemetn.addCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>detailsOfCompany</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,22 +74,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ComanyManagemetn.addDepartment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ComanyManagemetn.addDepartment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>departmentName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">auto_generated_DN </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,10 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ComanyManagemetn.addJob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jobTitle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,62 +102,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>auto_generated_JT_testinggggggggggggggggggggggggggggggggggggggggggg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TrainScheduling_ltrailways_addStuff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ComanyManagemetn.addStuff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>stuffName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>auto_generated_SN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>password</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>auto_generated_PWD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>realStuffName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>auto_generated_RSN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>stuffMail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>auto_generated_SM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>stuffPhoneNum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13659191907</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>schedulingInfo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -190,7 +138,79 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_generated_JT_testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_RSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_SN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13645541254</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test231120@126.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_updateCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.addCompany</t>
+  </si>
+  <si>
+    <t>CompanyManagement.addDepartment</t>
+  </si>
+  <si>
+    <t>CompanyManagement.addJob</t>
+  </si>
+  <si>
+    <t>CompanyManagement.addStuff</t>
+  </si>
+  <si>
+    <t>CompanyManagement.updateCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_generated_CN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_generated_CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -198,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +231,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -257,10 +284,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -273,9 +304,11 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -567,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -578,7 +611,7 @@
     <col min="1" max="1" width="35.875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" style="1" bestFit="1" customWidth="1"/>
@@ -620,10 +653,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -635,13 +668,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" ht="15.95" customHeight="1">
@@ -652,186 +685,229 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="8" spans="1:13" s="6" customFormat="1" ht="15.95" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="15.95" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="6" customFormat="1" ht="15.95" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="I14" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>37</v>
+      <c r="J15" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add 'remove_company' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -211,6 +211,30 @@
   </si>
   <si>
     <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_removeCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.removeCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRemove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,17 +624,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.25" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.625" style="1" bestFit="1" customWidth="1"/>
@@ -863,7 +887,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="15.95" customHeight="1">
+    <row r="17" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
@@ -883,7 +907,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="15.95" customHeight="1">
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
@@ -902,6 +926,41 @@
       <c r="F18" s="3" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="20" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update 'remove_company' and add 'update_department' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -234,7 +234,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TrainScheduling_ltrailways_updateDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.updateDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_generated_DN </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -624,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -955,12 +971,52 @@
         <v>51</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G21" s="5"/>
+    </row>
+    <row r="23" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add 'remove_department' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,11 +246,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">auto_generated_DN </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">auto_generated_DN </t>
+    <t>TrainScheduling_ltrailways_removeDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.removeDepartment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -640,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -766,7 +774,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -1009,14 +1017,49 @@
         <v>56</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add 'update_job' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -142,10 +142,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>auto_generated_JT_testing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>false</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -158,11 +154,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13645541254</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test231120@126.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_updateCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.addCompany</t>
+  </si>
+  <si>
+    <t>CompanyManagement.addDepartment</t>
+  </si>
+  <si>
+    <t>CompanyManagement.addJob</t>
+  </si>
+  <si>
+    <t>CompanyManagement.addStuff</t>
+  </si>
+  <si>
+    <t>CompanyManagement.updateCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_generated_CN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_generated_CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5</t>
+    <t>TrainScheduling_ltrailways_removeCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.removeCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRemove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_updateDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.updateDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_generated_DN </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -170,39 +246,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13645541254</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test231120@126.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TrainScheduling_ltrailways_updateCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CompanyManagement.addCompany</t>
-  </si>
-  <si>
-    <t>CompanyManagement.addDepartment</t>
-  </si>
-  <si>
-    <t>CompanyManagement.addJob</t>
-  </si>
-  <si>
-    <t>CompanyManagement.addStuff</t>
-  </si>
-  <si>
-    <t>CompanyManagement.updateCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>auto_generated_CN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>auto_generated_CD</t>
+    <t>TrainScheduling_ltrailways_removeDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.removeDepartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_updateJob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.updateJob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_generated_JT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -210,55 +278,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TrainScheduling_ltrailways_removeCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CompanyManagement.removeCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isRemove</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rowIndex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TrainScheduling_ltrailways_updateDepartment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CompanyManagement.updateDepartment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rowIndex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">auto_generated_DN </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TrainScheduling_ltrailways_removeDepartment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CompanyManagement.removeDepartment</t>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -648,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -716,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>7</v>
@@ -733,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -751,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>7</v>
@@ -771,10 +791,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -791,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>7</v>
@@ -814,16 +834,16 @@
         <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>20</v>
@@ -837,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>7</v>
@@ -878,48 +898,48 @@
         <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="B17" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>7</v>
@@ -928,76 +948,76 @@
         <v>9</v>
       </c>
       <c r="F17" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="B20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="D20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="6" t="s">
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="23" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>14</v>
@@ -1006,60 +1026,112 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
+    <row r="24" spans="1:8" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="15.95" customHeight="1">
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="15.95" customHeight="1">
       <c r="A26" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="E30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="5"/>
+      <c r="F30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add 'remove_job' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,6 +279,14 @@
   </si>
   <si>
     <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_removeJob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.removeJob</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -668,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -1132,6 +1140,41 @@
       <c r="H30" s="3" t="s">
         <v>66</v>
       </c>
+    </row>
+    <row r="32" spans="1:8" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add 'update_stuff' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="78">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,6 +287,42 @@
   </si>
   <si>
     <t>CompanyManagement.removeJob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_updateStuff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.updateStuff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rowIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13665541254</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test115@126.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -676,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -694,7 +730,7 @@
     <col min="8" max="8" width="20.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.75" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9" style="1"/>
@@ -1158,7 +1194,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="15.95" customHeight="1">
+    <row r="33" spans="1:12" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>67</v>
       </c>
@@ -1175,11 +1211,88 @@
         <v>51</v>
       </c>
       <c r="G33" s="5"/>
+    </row>
+    <row r="35" spans="1:12" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A35" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J15" r:id="rId1"/>
+    <hyperlink ref="H36" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'remove_stuff' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="80">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -323,6 +323,14 @@
   </si>
   <si>
     <t>test115@126.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_removeStuff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.removeStuff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -712,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -1287,6 +1295,41 @@
       <c r="L36" s="3" t="s">
         <v>75</v>
       </c>
+    </row>
+    <row r="38" spans="1:12" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A38" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add 'ubnt_configuration' automation script
</commit_message>
<xml_diff>
--- a/src/main/java/testData/testData.xlsx
+++ b/src/main/java/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="83">
   <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>CompanyManagement.removeStuff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrainScheduling_ltrailways_searchCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyManagement.searchCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>companyName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -720,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -1330,6 +1342,35 @@
         <v>51</v>
       </c>
       <c r="F39" s="5"/>
+    </row>
+    <row r="41" spans="1:12" s="6" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A41" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="3" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>